<commit_message>
Add and update two pool and maturation models
</commit_message>
<xml_diff>
--- a/Two_Pool_and_Maturation/Three_sensor.xlsx
+++ b/Two_Pool_and_Maturation/Three_sensor.xlsx
@@ -8,28 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espru\OneDrive\Documents\GitHub\SynapseModel\Two_Pool_and_Maturation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E760729-FC5D-4FA3-96E2-10E1B805438C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA8046F-2DD3-4BE7-B6C5-96BF2E018612}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="CDR" sheetId="1" r:id="rId1"/>
     <sheet name="Unpriming" sheetId="2" r:id="rId2"/>
-    <sheet name="37Priming" sheetId="3" r:id="rId3"/>
+    <sheet name="37Priming_Hill" sheetId="3" r:id="rId3"/>
+    <sheet name="37Priming_membrane_binding" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="b_1">CDR!$B$78</definedName>
     <definedName name="b_3">CDR!$B$79</definedName>
     <definedName name="b_7">CDR!$B$80</definedName>
-    <definedName name="CDR">CDR!$B$82</definedName>
+    <definedName name="CDI">CDR!$B$84</definedName>
+    <definedName name="CDR">CDR!$B$83</definedName>
     <definedName name="k_off_1">CDR!$B$71</definedName>
     <definedName name="k_off_3">CDR!$B$72</definedName>
     <definedName name="k_off_7">CDR!$B$73</definedName>
     <definedName name="k_on_1">CDR!$B$68</definedName>
     <definedName name="k_on_3">CDR!$B$69</definedName>
     <definedName name="k_on_7">CDR!$B$70</definedName>
+    <definedName name="k_prime_basal">CDR!$B$85</definedName>
     <definedName name="k_refill">CDR!$B$81</definedName>
-    <definedName name="k_unprime">CDR!$B$83</definedName>
+    <definedName name="k_unfill">CDR!$B$82</definedName>
+    <definedName name="k_unprime">CDR!$B$85</definedName>
+    <definedName name="k_unprime_basal">CDR!$B$86</definedName>
     <definedName name="L_plus">CDR!$B$74</definedName>
     <definedName name="O">CDR!$B$75</definedName>
     <definedName name="S">CDR!$B$77</definedName>
@@ -52,8 +57,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="105">
   <si>
     <t>e00</t>
   </si>
@@ -334,9 +361,6 @@
     <t>Fused</t>
   </si>
   <si>
-    <t>k_unprime</t>
-  </si>
-  <si>
     <t>Fitted</t>
   </si>
   <si>
@@ -359,6 +383,18 @@
   </si>
   <si>
     <t>empty</t>
+  </si>
+  <si>
+    <t>k_prime_basal</t>
+  </si>
+  <si>
+    <t>k_unprime_basal</t>
+  </si>
+  <si>
+    <t>k_unfill</t>
+  </si>
+  <si>
+    <t>CDI</t>
   </si>
 </sst>
 </file>
@@ -395,7 +431,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,12 +530,50 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.5999938962981"/>
+        <fgColor theme="5" tint="0.59996337778863"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.24994659260842"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.49995422223579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.24994659260842"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="104">
+  <borders count="236">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -616,11 +690,141 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="277">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true"/>
@@ -685,8 +889,29 @@
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="true" applyFill="true" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="true" applyAlignment="true">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="true"/>
@@ -787,6 +1012,138 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="101" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="102" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="103" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="104" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="105" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="106" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="107" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="108" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="109" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="110" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="111" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="112" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="113" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="114" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="115" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="116" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="117" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="118" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="119" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="120" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="121" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="122" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="123" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="124" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="125" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="126" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="127" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="128" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="129" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="130" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="131" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="132" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="133" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="134" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="135" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="136" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="137" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="138" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="139" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="140" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="141" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="142" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="143" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="144" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="145" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="146" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="147" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="148" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="149" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="150" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="151" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="152" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="153" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="154" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="155" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="156" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="157" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="158" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="159" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="160" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="161" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="162" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="163" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="164" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="165" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="166" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="167" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="168" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="169" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="170" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="171" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="172" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="173" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="174" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="175" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="176" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="177" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="178" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="179" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="180" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="181" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="182" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="183" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="184" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="185" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="186" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="187" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="188" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="189" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="190" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="191" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="192" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="193" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="194" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="195" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="196" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="197" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="198" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="199" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="200" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="201" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="202" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="203" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="204" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="205" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="206" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="207" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="208" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="209" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="210" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="211" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="212" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="213" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="214" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="215" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="216" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="217" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="218" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="219" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="220" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="221" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="222" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="223" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="224" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="225" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="226" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="227" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="228" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="229" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="230" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="231" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="232" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="233" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="234" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="235" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -795,6 +1152,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFCC66FF"/>
       <color rgb="FFCCFF33"/>
     </mruColors>
   </colors>
@@ -1106,16 +1464,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3230F13-07AE-4036-B715-09A3C5AF7ED4}">
-  <dimension ref="A1:DZ83"/>
+  <dimension ref="A1:DZ86"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:P2"/>
+    <sheetView tabSelected="true" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="AG67" sqref="AG67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" customWidth="true"/>
-    <col min="2" max="2" width="7.140625" customWidth="true"/>
+    <col min="1" max="1" width="15" customWidth="true"/>
+    <col min="2" max="2" width="8.7109375" customWidth="true"/>
     <col min="3" max="3" width="15" customWidth="true"/>
     <col min="12" max="12" width="9.140625" customWidth="true"/>
   </cols>
@@ -1545,221 +1903,168 @@
       <c r="J2" s="6">
         <v>0</v>
       </c>
-      <c r="K2" s="8">
-        <f>L_plus</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="L2" s="8">
-        <f>L_plus*O</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="M2" s="8">
-        <f>L_plus*O^2</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="N2" s="8">
-        <f>L_plus*O^3</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="O2" s="8">
-        <f>L_plus*O^4</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="P2" s="8">
-        <f>L_plus*O^5</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="Q2" s="8">
-        <f>L_plus*S</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="R2" s="8">
-        <f>L_plus*O*S</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="S2" s="8">
-        <f>L_plus*O^2*S</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="T2" s="8">
-        <f>L_plus*O^3*S</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="U2" s="8">
-        <f>L_plus*O^4*S</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="V2" s="8">
-        <f>L_plus*O^5*S</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="W2" s="8">
-        <f>L_plus*S^2</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="X2" s="8">
-        <f>L_plus*O*S^2</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="Y2" s="8">
-        <f>L_plus*O^2*S^2</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="Z2" s="8">
-        <f>L_plus*O^3*S^2</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="AA2" s="8">
-        <f>L_plus*O^4*S^2</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="AB2" s="8">
-        <f>L_plus*O^5*S^2</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="AC2" s="8">
-        <f>L_plus*T</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="AD2" s="8">
-        <f>L_plus*O*T</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="AE2" s="8">
-        <f>L_plus*O^2*T</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="AF2" s="8">
-        <f>L_plus*O^3*T</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="AG2" s="8">
-        <f>L_plus*O^4*T</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="AH2" s="8">
-        <f>L_plus*O^5*T</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="AI2" s="8">
-        <f>L_plus*T^2</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="AJ2" s="8">
-        <f>L_plus*O*T^2</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="AK2" s="8">
-        <f>L_plus*O^2*T^2</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="AL2" s="8">
-        <f>L_plus*O^3*T^2</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="AM2" s="8">
-        <f>L_plus*O^4*T^2</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="AN2" s="8">
-        <f>L_plus*O^5*T^2</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="AO2" s="8">
-        <f>L_plus*T*S</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="AP2" s="8">
-        <f>L_plus*O*T*S</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="AQ2" s="8">
-        <f>L_plus*O^2*T*S</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="AR2" s="8">
-        <f>L_plus*O^3*T*S</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="AS2" s="8">
-        <f>L_plus*O^4*T*S</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="AT2" s="8">
-        <f>L_plus*O^5*T*S</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="AU2" s="8">
-        <f>L_plus*T^2*S</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="AV2" s="8">
-        <f>L_plus*O*T^2*S</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="AW2" s="8">
-        <f>L_plus*O^2*T^2*S</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="AX2" s="8">
-        <f>L_plus*O^3*T^2*S</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="AY2" s="8">
-        <f>L_plus*O^4*T^2*S</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="AZ2" s="8">
-        <f>L_plus*O^5*T^2*S</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="BA2" s="8">
-        <f>L_plus*T*S^2</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="BB2" s="8">
-        <f>L_plus*O*T*S^2</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="BC2" s="8">
-        <f>L_plus*O^2*T*S^2</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="BD2" s="8">
-        <f>L_plus*O^3*T*S^2</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="BE2" s="8">
-        <f>L_plus*O^4*T*S^2</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="BF2" s="8">
-        <f>L_plus*O^5*T*S^2</f>
-        <v>6.0000017014813656</v>
-      </c>
-      <c r="BG2" s="8">
-        <f>L_plus*T^2*S^2</f>
-        <v>3.4999999999999998E-7</v>
-      </c>
-      <c r="BH2" s="8">
-        <f>L_plus*O*T^2*S^2</f>
-        <v>9.7922999999999994E-6</v>
-      </c>
-      <c r="BI2" s="8">
-        <f>L_plus*O^2*T^2*S^2</f>
-        <v>2.7396896940000003E-4</v>
-      </c>
-      <c r="BJ2" s="8">
-        <f>L_plus*O^3*T^2*S^2</f>
-        <v>7.6651038258732001E-3</v>
-      </c>
-      <c r="BK2" s="8">
-        <f>L_plus*O^4*T^2*S^2</f>
-        <v>0.2144542748402804</v>
-      </c>
-      <c r="BL2" s="8">
-        <f>L_plus*O^5*T^2*S^2</f>
-        <v>6.0000017014813656</v>
+      <c r="K2" s="44">
+        <f>k_unfill</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="6">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0</v>
+      </c>
+      <c r="T2" s="6">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6">
+        <v>0</v>
+      </c>
+      <c r="W2" s="6">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AW2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AX2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AY2" s="6">
+        <v>0</v>
+      </c>
+      <c r="AZ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BA2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BC2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BD2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BE2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BF2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BG2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BH2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BI2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BJ2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BK2" s="6">
+        <v>0</v>
+      </c>
+      <c r="BL2" s="6">
+        <v>0</v>
       </c>
       <c r="BM2" s="6">
         <v>0</v>
@@ -2047,7 +2352,8 @@
       <c r="AB3" s="6">
         <v>0</v>
       </c>
-      <c r="AC3" s="6">
+      <c r="AC3" s="44">
+        <f>k_unfill</f>
         <v>0</v>
       </c>
       <c r="AD3" s="6">
@@ -2163,7 +2469,7 @@
       </c>
       <c r="BO3" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BP3" s="4">
         <v>0</v>
@@ -2459,7 +2765,8 @@
       <c r="AH4" s="6">
         <v>0</v>
       </c>
-      <c r="AI4" s="6">
+      <c r="AI4" s="44">
+        <f>k_unfill</f>
         <v>0</v>
       </c>
       <c r="AJ4" s="6">
@@ -2560,7 +2867,7 @@
       </c>
       <c r="BP4" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BQ4" s="4">
         <v>0</v>
@@ -2800,7 +3107,8 @@
       <c r="P5" s="6">
         <v>0</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="44" cm="1">
+        <f t="array" ref="Q5">k_unfill*CDI</f>
         <v>0</v>
       </c>
       <c r="R5" s="6">
@@ -2952,7 +3260,7 @@
       </c>
       <c r="BO5" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BP5" s="6">
         <v>0</v>
@@ -3212,7 +3520,8 @@
       <c r="V6" s="6">
         <v>0</v>
       </c>
-      <c r="W6" s="6">
+      <c r="W6" s="44">
+        <f>k_unfill*CDI^2</f>
         <v>0</v>
       </c>
       <c r="X6" s="6">
@@ -3355,7 +3664,7 @@
       </c>
       <c r="BR6" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BS6" s="4">
         <v>0</v>
@@ -3661,7 +3970,8 @@
       <c r="AN7" s="6">
         <v>0</v>
       </c>
-      <c r="AO7" s="6">
+      <c r="AO7" s="44" cm="1">
+        <f t="array" ref="AO7">k_unfill*CDI</f>
         <v>0</v>
       </c>
       <c r="AP7" s="6">
@@ -3744,14 +4054,14 @@
       </c>
       <c r="BP7" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BQ7" s="6">
         <v>0</v>
       </c>
       <c r="BR7" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BS7" s="6">
         <v>0</v>
@@ -4092,7 +4402,8 @@
       <c r="AZ8" s="6">
         <v>0</v>
       </c>
-      <c r="BA8" s="6">
+      <c r="BA8" s="44">
+        <f>k_unfill*CDI^2</f>
         <v>0</v>
       </c>
       <c r="BB8" s="6">
@@ -4148,11 +4459,11 @@
       </c>
       <c r="BS8" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BT8" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BU8" s="4">
         <v>0</v>
@@ -4469,7 +4780,8 @@
       <c r="AT9" s="6">
         <v>0</v>
       </c>
-      <c r="AU9" s="6">
+      <c r="AU9" s="44" cm="1">
+        <f t="array" ref="AU9">k_unfill*CDI</f>
         <v>0</v>
       </c>
       <c r="AV9" s="6">
@@ -4537,7 +4849,7 @@
       </c>
       <c r="BQ9" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BR9" s="6">
         <v>0</v>
@@ -4547,7 +4859,7 @@
       </c>
       <c r="BT9" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BU9" s="6">
         <v>0</v>
@@ -4899,7 +5211,8 @@
       <c r="BF10" s="6">
         <v>0</v>
       </c>
-      <c r="BG10" s="6">
+      <c r="BG10" s="44">
+        <f>k_unfill*CDI^2</f>
         <v>0</v>
       </c>
       <c r="BH10" s="6">
@@ -4943,11 +5256,11 @@
       </c>
       <c r="BU10" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BV10" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BW10" s="4">
         <v>0</v>
@@ -5124,7 +5437,7 @@
       </c>
       <c r="B11" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -7508,7 +7821,7 @@
       </c>
       <c r="E17" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -7725,7 +8038,7 @@
       </c>
       <c r="BX17" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BY17" s="6">
         <v>0</v>
@@ -8124,7 +8437,7 @@
       </c>
       <c r="BY18" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BZ18" s="6">
         <v>0</v>
@@ -8524,7 +8837,7 @@
       </c>
       <c r="BZ19" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CA19" s="6">
         <v>0</v>
@@ -8924,7 +9237,7 @@
       </c>
       <c r="CA20" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CB20" s="6">
         <v>0</v>
@@ -9324,7 +9637,7 @@
       </c>
       <c r="CB21" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CC21" s="6">
         <v>0</v>
@@ -9723,7 +10036,7 @@
       </c>
       <c r="CC22" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CD22" s="6">
         <v>0</v>
@@ -9892,7 +10205,7 @@
       </c>
       <c r="F23" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -10123,7 +10436,7 @@
       </c>
       <c r="CD23" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CE23" s="6">
         <v>0</v>
@@ -10521,7 +10834,7 @@
       </c>
       <c r="CE24" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CF24" s="6">
         <v>0</v>
@@ -10920,7 +11233,7 @@
       </c>
       <c r="CF25" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CG25" s="6">
         <v>0</v>
@@ -11319,7 +11632,7 @@
       </c>
       <c r="CG26" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CH26" s="6">
         <v>0</v>
@@ -11718,7 +12031,7 @@
       </c>
       <c r="CH27" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CI27" s="6">
         <v>0</v>
@@ -12116,7 +12429,7 @@
       </c>
       <c r="CI28" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CJ28" s="6">
         <v>0</v>
@@ -12258,7 +12571,7 @@
       </c>
       <c r="C29" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="D29" s="6">
         <v>0</v>
@@ -12481,7 +12794,7 @@
       </c>
       <c r="BX29" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BY29" s="6">
         <v>0</v>
@@ -12880,7 +13193,7 @@
       </c>
       <c r="BY30" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BZ30" s="6">
         <v>0</v>
@@ -13280,7 +13593,7 @@
       </c>
       <c r="BZ31" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CA31" s="6">
         <v>0</v>
@@ -13680,7 +13993,7 @@
       </c>
       <c r="CA32" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="6">
         <v>0</v>
@@ -14080,7 +14393,7 @@
       </c>
       <c r="CB33" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CC33" s="6">
         <v>0</v>
@@ -14479,7 +14792,7 @@
       </c>
       <c r="CC34" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CD34" s="6">
         <v>0</v>
@@ -14642,7 +14955,7 @@
       </c>
       <c r="D35" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
@@ -14915,7 +15228,7 @@
       </c>
       <c r="CP35" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CQ35" s="6">
         <v>0</v>
@@ -15313,7 +15626,7 @@
       </c>
       <c r="CQ36" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CR36" s="6">
         <v>0</v>
@@ -15712,7 +16025,7 @@
       </c>
       <c r="CR37" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CS37" s="6">
         <v>0</v>
@@ -16111,7 +16424,7 @@
       </c>
       <c r="CS38" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CT38" s="6">
         <v>0</v>
@@ -16510,7 +16823,7 @@
       </c>
       <c r="CT39" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CU39" s="6">
         <v>0</v>
@@ -16908,7 +17221,7 @@
       </c>
       <c r="CU40" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CV40" s="6">
         <v>0</v>
@@ -17026,7 +17339,7 @@
       </c>
       <c r="G41" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H41" s="6">
         <v>0</v>
@@ -17255,7 +17568,7 @@
       </c>
       <c r="CD41" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CE41" s="6">
         <v>0</v>
@@ -17292,7 +17605,7 @@
       </c>
       <c r="CP41" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CQ41" s="6">
         <v>0</v>
@@ -17655,7 +17968,7 @@
       </c>
       <c r="CE42" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CF42" s="6">
         <v>0</v>
@@ -17692,7 +18005,7 @@
       </c>
       <c r="CQ42" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CR42" s="6">
         <v>0</v>
@@ -18056,7 +18369,7 @@
       </c>
       <c r="CF43" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CG43" s="6">
         <v>0</v>
@@ -18093,7 +18406,7 @@
       </c>
       <c r="CR43" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CS43" s="6">
         <v>0</v>
@@ -18457,7 +18770,7 @@
       </c>
       <c r="CG44" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CH44" s="6">
         <v>0</v>
@@ -18494,7 +18807,7 @@
       </c>
       <c r="CS44" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CT44" s="6">
         <v>0</v>
@@ -18858,7 +19171,7 @@
       </c>
       <c r="CH45" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CI45" s="6">
         <v>0</v>
@@ -18895,7 +19208,7 @@
       </c>
       <c r="CT45" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CU45" s="6">
         <v>0</v>
@@ -19258,7 +19571,7 @@
       </c>
       <c r="CI46" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CJ46" s="6">
         <v>0</v>
@@ -19295,7 +19608,7 @@
       </c>
       <c r="CU46" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CV46" s="6">
         <v>0</v>
@@ -19419,7 +19732,7 @@
       </c>
       <c r="I47" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="J47" s="6">
         <v>0</v>
@@ -19695,7 +20008,7 @@
       </c>
       <c r="CV47" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CW47" s="6">
         <v>0</v>
@@ -19714,7 +20027,7 @@
       </c>
       <c r="DB47" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DC47" s="6">
         <v>0</v>
@@ -20094,7 +20407,7 @@
       </c>
       <c r="CW48" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CX48" s="6">
         <v>0</v>
@@ -20113,7 +20426,7 @@
       </c>
       <c r="DC48" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DD48" s="6">
         <v>0</v>
@@ -20494,7 +20807,7 @@
       </c>
       <c r="CX49" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CY49" s="6">
         <v>0</v>
@@ -20513,7 +20826,7 @@
       </c>
       <c r="DD49" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DE49" s="6">
         <v>0</v>
@@ -20894,7 +21207,7 @@
       </c>
       <c r="CY50" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CZ50" s="6">
         <v>0</v>
@@ -20913,7 +21226,7 @@
       </c>
       <c r="DE50" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DF50" s="6">
         <v>0</v>
@@ -21294,7 +21607,7 @@
       </c>
       <c r="CZ51" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="DA51" s="6">
         <v>0</v>
@@ -21313,7 +21626,7 @@
       </c>
       <c r="DF51" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DG51" s="6">
         <v>0</v>
@@ -21693,7 +22006,7 @@
       </c>
       <c r="DA52" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="DB52" s="6">
         <v>0</v>
@@ -21712,7 +22025,7 @@
       </c>
       <c r="DG52" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DH52" s="6">
         <v>0</v>
@@ -21797,7 +22110,7 @@
       </c>
       <c r="H53" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="I53" s="6">
         <v>0</v>
@@ -22040,7 +22353,7 @@
       </c>
       <c r="CJ53" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CK53" s="6">
         <v>0</v>
@@ -22095,7 +22408,7 @@
       </c>
       <c r="DB53" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DC53" s="6">
         <v>0</v>
@@ -22439,7 +22752,7 @@
       </c>
       <c r="CK54" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CL54" s="6">
         <v>0</v>
@@ -22494,7 +22807,7 @@
       </c>
       <c r="DC54" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DD54" s="6">
         <v>0</v>
@@ -22839,7 +23152,7 @@
       </c>
       <c r="CL55" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CM55" s="6">
         <v>0</v>
@@ -22894,7 +23207,7 @@
       </c>
       <c r="DD55" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DE55" s="6">
         <v>0</v>
@@ -23239,7 +23552,7 @@
       </c>
       <c r="CM56" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CN56" s="6">
         <v>0</v>
@@ -23294,7 +23607,7 @@
       </c>
       <c r="DE56" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DF56" s="6">
         <v>0</v>
@@ -23639,7 +23952,7 @@
       </c>
       <c r="CN57" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CO57" s="6">
         <v>0</v>
@@ -23694,7 +24007,7 @@
       </c>
       <c r="DF57" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DG57" s="6">
         <v>0</v>
@@ -24038,7 +24351,7 @@
       </c>
       <c r="CO58" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CP58" s="6">
         <v>0</v>
@@ -24093,7 +24406,7 @@
       </c>
       <c r="DG58" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DH58" s="6">
         <v>0</v>
@@ -24184,7 +24497,7 @@
       </c>
       <c r="J59" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="K59" s="6">
         <v>0</v>
@@ -24492,7 +24805,7 @@
       </c>
       <c r="DH59" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DI59" s="6">
         <v>0</v>
@@ -24511,7 +24824,7 @@
       </c>
       <c r="DN59" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DO59" s="6">
         <v>0</v>
@@ -24890,7 +25203,7 @@
       </c>
       <c r="DI60" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DJ60" s="6">
         <v>0</v>
@@ -24909,7 +25222,7 @@
       </c>
       <c r="DO60" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DP60" s="6">
         <v>0</v>
@@ -25289,7 +25602,7 @@
       </c>
       <c r="DJ61" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DK61" s="6">
         <v>0</v>
@@ -25308,7 +25621,7 @@
       </c>
       <c r="DP61" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DQ61" s="6">
         <v>0</v>
@@ -25688,7 +26001,7 @@
       </c>
       <c r="DK62" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DL62" s="6">
         <v>0</v>
@@ -25707,7 +26020,7 @@
       </c>
       <c r="DQ62" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DR62" s="6">
         <v>0</v>
@@ -26087,7 +26400,7 @@
       </c>
       <c r="DL63" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DM63" s="6">
         <v>0</v>
@@ -26106,7 +26419,7 @@
       </c>
       <c r="DR63" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DS63" s="6">
         <v>0</v>
@@ -26485,7 +26798,7 @@
       </c>
       <c r="DM64" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DN64" s="6">
         <v>0</v>
@@ -26504,7 +26817,7 @@
       </c>
       <c r="DS64" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DT64" s="6">
         <v>0</v>
@@ -27029,7 +27342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" x14ac:dyDescent="0.25">
+    <row r="67" ht="30" x14ac:dyDescent="0.25">
       <c r="A67" s="14" t="s">
         <v>63</v>
       </c>
@@ -27045,8 +27358,8 @@
       <c r="A68" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="B68" s="29">
-        <v>140000</v>
+      <c r="B68" s="37">
+        <v>550000</v>
       </c>
       <c r="C68" s="16" t="s">
         <v>84</v>
@@ -27057,8 +27370,8 @@
       <c r="A69" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B69" s="29">
-        <v>300000</v>
+      <c r="B69" s="37">
+        <v>0</v>
       </c>
       <c r="C69" s="16" t="s">
         <v>87</v>
@@ -27069,8 +27382,8 @@
       <c r="A70" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B70" s="29">
-        <v>7333</v>
+      <c r="B70" s="37">
+        <v>0</v>
       </c>
       <c r="C70" s="16" t="s">
         <v>88</v>
@@ -27203,26 +27516,50 @@
         <v>82</v>
       </c>
       <c r="B81" s="29">
-        <v>0.001</v>
+        <v>0.0028999999999999998</v>
       </c>
     </row>
     <row r="82" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>83</v>
-      </c>
-      <c r="B82" s="29">
-        <v>1</v>
-      </c>
-      <c r="C82" s="16" t="s">
-        <v>94</v>
+      <c r="A82" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82" s="42">
+        <v>0</v>
       </c>
     </row>
     <row r="83" x14ac:dyDescent="0.25">
-      <c r="A83" s="28" t="s">
-        <v>93</v>
+      <c r="A83" s="24" t="s">
+        <v>83</v>
       </c>
       <c r="B83" s="29">
         <v>1</v>
+      </c>
+      <c r="C83" s="16" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" x14ac:dyDescent="0.25">
+      <c r="A84" s="43" t="s">
+        <v>104</v>
+      </c>
+      <c r="B84" s="42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="85" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
+        <v>101</v>
+      </c>
+      <c r="B85" s="36">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="86" x14ac:dyDescent="0.25">
+      <c r="A86" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B86" s="38">
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>
@@ -27234,8 +27571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8DB6E53-8373-42EB-9501-81D344630E67}">
   <dimension ref="A1:DZ65"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="K1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28229,7 +28566,7 @@
       </c>
       <c r="BO3" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BP3" s="4">
         <v>0</v>
@@ -28626,7 +28963,7 @@
       </c>
       <c r="BP4" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BQ4" s="4">
         <v>0</v>
@@ -29018,7 +29355,7 @@
       </c>
       <c r="BO5" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BP5" s="6">
         <v>0</v>
@@ -29421,7 +29758,7 @@
       </c>
       <c r="BR6" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BS6" s="4">
         <v>0</v>
@@ -29810,14 +30147,14 @@
       </c>
       <c r="BP7" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BQ7" s="6">
         <v>0</v>
       </c>
       <c r="BR7" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BS7" s="6">
         <v>0</v>
@@ -30214,11 +30551,11 @@
       </c>
       <c r="BS8" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BT8" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BU8" s="4">
         <v>0</v>
@@ -30603,7 +30940,7 @@
       </c>
       <c r="BQ9" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BR9" s="6">
         <v>0</v>
@@ -30613,7 +30950,7 @@
       </c>
       <c r="BT9" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BU9" s="6">
         <v>0</v>
@@ -31009,11 +31346,11 @@
       </c>
       <c r="BU10" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="BV10" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="BW10" s="4">
         <v>0</v>
@@ -31190,7 +31527,7 @@
       </c>
       <c r="B11" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="C11" s="6">
         <v>0</v>
@@ -33574,7 +33911,7 @@
       </c>
       <c r="E17" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="F17" s="6">
         <v>0</v>
@@ -33791,7 +34128,7 @@
       </c>
       <c r="BX17" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BY17" s="6">
         <v>0</v>
@@ -34190,7 +34527,7 @@
       </c>
       <c r="BY18" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="BZ18" s="6">
         <v>0</v>
@@ -34590,7 +34927,7 @@
       </c>
       <c r="BZ19" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CA19" s="6">
         <v>0</v>
@@ -34990,7 +35327,7 @@
       </c>
       <c r="CA20" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CB20" s="6">
         <v>0</v>
@@ -35390,7 +35727,7 @@
       </c>
       <c r="CB21" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CC21" s="6">
         <v>0</v>
@@ -35789,7 +36126,7 @@
       </c>
       <c r="CC22" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CD22" s="6">
         <v>0</v>
@@ -35958,7 +36295,7 @@
       </c>
       <c r="F23" s="11">
         <f>k_refill</f>
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="G23" s="6">
         <v>0</v>
@@ -36189,7 +36526,7 @@
       </c>
       <c r="CD23" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CE23" s="6">
         <v>0</v>
@@ -36587,7 +36924,7 @@
       </c>
       <c r="CE24" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CF24" s="6">
         <v>0</v>
@@ -36986,7 +37323,7 @@
       </c>
       <c r="CF25" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CG25" s="6">
         <v>0</v>
@@ -37385,7 +37722,7 @@
       </c>
       <c r="CG26" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CH26" s="6">
         <v>0</v>
@@ -37784,7 +38121,7 @@
       </c>
       <c r="CH27" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CI27" s="6">
         <v>0</v>
@@ -38182,7 +38519,7 @@
       </c>
       <c r="CI28" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="CJ28" s="6">
         <v>0</v>
@@ -38324,7 +38661,7 @@
       </c>
       <c r="C29" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="D29" s="6">
         <v>0</v>
@@ -38547,7 +38884,7 @@
       </c>
       <c r="BX29" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BY29" s="6">
         <v>0</v>
@@ -38946,7 +39283,7 @@
       </c>
       <c r="BY30" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="BZ30" s="6">
         <v>0</v>
@@ -39346,7 +39683,7 @@
       </c>
       <c r="BZ31" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CA31" s="6">
         <v>0</v>
@@ -39746,7 +40083,7 @@
       </c>
       <c r="CA32" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CB32" s="6">
         <v>0</v>
@@ -40146,7 +40483,7 @@
       </c>
       <c r="CB33" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CC33" s="6">
         <v>0</v>
@@ -40545,7 +40882,7 @@
       </c>
       <c r="CC34" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CD34" s="6">
         <v>0</v>
@@ -40708,7 +41045,7 @@
       </c>
       <c r="D35" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="E35" s="6">
         <v>0</v>
@@ -40981,7 +41318,7 @@
       </c>
       <c r="CP35" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CQ35" s="6">
         <v>0</v>
@@ -41379,7 +41716,7 @@
       </c>
       <c r="CQ36" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CR36" s="6">
         <v>0</v>
@@ -41778,7 +42115,7 @@
       </c>
       <c r="CR37" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CS37" s="6">
         <v>0</v>
@@ -42177,7 +42514,7 @@
       </c>
       <c r="CS38" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CT38" s="6">
         <v>0</v>
@@ -42576,7 +42913,7 @@
       </c>
       <c r="CT39" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CU39" s="6">
         <v>0</v>
@@ -42974,7 +43311,7 @@
       </c>
       <c r="CU40" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="CV40" s="6">
         <v>0</v>
@@ -43092,7 +43429,7 @@
       </c>
       <c r="G41" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="H41" s="6">
         <v>0</v>
@@ -43321,7 +43658,7 @@
       </c>
       <c r="CD41" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CE41" s="6">
         <v>0</v>
@@ -43358,7 +43695,7 @@
       </c>
       <c r="CP41" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CQ41" s="6">
         <v>0</v>
@@ -43721,7 +44058,7 @@
       </c>
       <c r="CE42" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CF42" s="6">
         <v>0</v>
@@ -43758,7 +44095,7 @@
       </c>
       <c r="CQ42" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CR42" s="6">
         <v>0</v>
@@ -44122,7 +44459,7 @@
       </c>
       <c r="CF43" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CG43" s="6">
         <v>0</v>
@@ -44159,7 +44496,7 @@
       </c>
       <c r="CR43" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CS43" s="6">
         <v>0</v>
@@ -44523,7 +44860,7 @@
       </c>
       <c r="CG44" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CH44" s="6">
         <v>0</v>
@@ -44560,7 +44897,7 @@
       </c>
       <c r="CS44" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CT44" s="6">
         <v>0</v>
@@ -44924,7 +45261,7 @@
       </c>
       <c r="CH45" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CI45" s="6">
         <v>0</v>
@@ -44961,7 +45298,7 @@
       </c>
       <c r="CT45" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CU45" s="6">
         <v>0</v>
@@ -45324,7 +45661,7 @@
       </c>
       <c r="CI46" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CJ46" s="6">
         <v>0</v>
@@ -45361,7 +45698,7 @@
       </c>
       <c r="CU46" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CV46" s="6">
         <v>0</v>
@@ -45485,7 +45822,7 @@
       </c>
       <c r="I47" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="J47" s="6">
         <v>0</v>
@@ -45761,7 +46098,7 @@
       </c>
       <c r="CV47" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CW47" s="6">
         <v>0</v>
@@ -45780,7 +46117,7 @@
       </c>
       <c r="DB47" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DC47" s="6">
         <v>0</v>
@@ -46160,7 +46497,7 @@
       </c>
       <c r="CW48" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CX48" s="6">
         <v>0</v>
@@ -46179,7 +46516,7 @@
       </c>
       <c r="DC48" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DD48" s="6">
         <v>0</v>
@@ -46560,7 +46897,7 @@
       </c>
       <c r="CX49" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CY49" s="6">
         <v>0</v>
@@ -46579,7 +46916,7 @@
       </c>
       <c r="DD49" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DE49" s="6">
         <v>0</v>
@@ -46960,7 +47297,7 @@
       </c>
       <c r="CY50" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="CZ50" s="6">
         <v>0</v>
@@ -46979,7 +47316,7 @@
       </c>
       <c r="DE50" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DF50" s="6">
         <v>0</v>
@@ -47360,7 +47697,7 @@
       </c>
       <c r="CZ51" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="DA51" s="6">
         <v>0</v>
@@ -47379,7 +47716,7 @@
       </c>
       <c r="DF51" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DG51" s="6">
         <v>0</v>
@@ -47759,7 +48096,7 @@
       </c>
       <c r="DA52" s="10">
         <f>2*k_on_7</f>
-        <v>14666</v>
+        <v>0</v>
       </c>
       <c r="DB52" s="6">
         <v>0</v>
@@ -47778,7 +48115,7 @@
       </c>
       <c r="DG52" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DH52" s="6">
         <v>0</v>
@@ -47863,7 +48200,7 @@
       </c>
       <c r="H53" s="11">
         <f>k_refill*CDR</f>
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="I53" s="6">
         <v>0</v>
@@ -48106,7 +48443,7 @@
       </c>
       <c r="CJ53" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CK53" s="6">
         <v>0</v>
@@ -48161,7 +48498,7 @@
       </c>
       <c r="DB53" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DC53" s="6">
         <v>0</v>
@@ -48505,7 +48842,7 @@
       </c>
       <c r="CK54" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CL54" s="6">
         <v>0</v>
@@ -48560,7 +48897,7 @@
       </c>
       <c r="DC54" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DD54" s="6">
         <v>0</v>
@@ -48905,7 +49242,7 @@
       </c>
       <c r="CL55" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CM55" s="6">
         <v>0</v>
@@ -48960,7 +49297,7 @@
       </c>
       <c r="DD55" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DE55" s="6">
         <v>0</v>
@@ -49305,7 +49642,7 @@
       </c>
       <c r="CM56" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CN56" s="6">
         <v>0</v>
@@ -49360,7 +49697,7 @@
       </c>
       <c r="DE56" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DF56" s="6">
         <v>0</v>
@@ -49705,7 +50042,7 @@
       </c>
       <c r="CN57" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CO57" s="6">
         <v>0</v>
@@ -49760,7 +50097,7 @@
       </c>
       <c r="DF57" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DG57" s="6">
         <v>0</v>
@@ -50104,7 +50441,7 @@
       </c>
       <c r="CO58" s="9">
         <f>2*k_on_3</f>
-        <v>600000</v>
+        <v>0</v>
       </c>
       <c r="CP58" s="6">
         <v>0</v>
@@ -50159,7 +50496,7 @@
       </c>
       <c r="DG58" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DH58" s="6">
         <v>0</v>
@@ -50250,7 +50587,7 @@
       </c>
       <c r="J59" s="11">
         <f>k_refill*CDR^2</f>
-        <v>0.9</v>
+        <v>0</v>
       </c>
       <c r="K59" s="6">
         <v>0</v>
@@ -50558,7 +50895,7 @@
       </c>
       <c r="DH59" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DI59" s="6">
         <v>0</v>
@@ -50577,7 +50914,7 @@
       </c>
       <c r="DN59" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DO59" s="6">
         <v>0</v>
@@ -50956,7 +51293,7 @@
       </c>
       <c r="DI60" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DJ60" s="6">
         <v>0</v>
@@ -50975,7 +51312,7 @@
       </c>
       <c r="DO60" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DP60" s="6">
         <v>0</v>
@@ -51355,7 +51692,7 @@
       </c>
       <c r="DJ61" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DK61" s="6">
         <v>0</v>
@@ -51374,7 +51711,7 @@
       </c>
       <c r="DP61" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DQ61" s="6">
         <v>0</v>
@@ -51754,7 +52091,7 @@
       </c>
       <c r="DK62" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DL62" s="6">
         <v>0</v>
@@ -51773,7 +52110,7 @@
       </c>
       <c r="DQ62" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DR62" s="6">
         <v>0</v>
@@ -52153,7 +52490,7 @@
       </c>
       <c r="DL63" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DM63" s="6">
         <v>0</v>
@@ -52172,7 +52509,7 @@
       </c>
       <c r="DR63" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DS63" s="6">
         <v>0</v>
@@ -52551,7 +52888,7 @@
       </c>
       <c r="DM64" s="10">
         <f>k_on_7</f>
-        <v>7333</v>
+        <v>0</v>
       </c>
       <c r="DN64" s="6">
         <v>0</v>
@@ -52570,7 +52907,7 @@
       </c>
       <c r="DS64" s="9">
         <f>k_on_3</f>
-        <v>300000</v>
+        <v>0</v>
       </c>
       <c r="DT64" s="6">
         <v>0</v>
@@ -53104,8 +53441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FD513DA-E622-4A35-86DF-1F12F970B9E6}">
   <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53118,25 +53455,25 @@
         <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="F1" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="G1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="I1" s="31" t="s">
         <v>99</v>
-      </c>
-      <c r="I1" s="31" t="s">
-        <v>100</v>
       </c>
       <c r="K1" s="30" t="s">
         <v>91</v>
@@ -53145,25 +53482,25 @@
         <v>92</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="O1" s="31" t="s">
+      <c r="P1" s="31" t="s">
         <v>96</v>
       </c>
-      <c r="P1" s="31" t="s">
+      <c r="Q1" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="31" t="s">
+      <c r="R1" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="R1" s="31" t="s">
+      <c r="S1" s="31" t="s">
         <v>99</v>
-      </c>
-      <c r="S1" s="31" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
@@ -53230,7 +53567,7 @@
     </row>
     <row r="3" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B3" s="6">
         <v>0</v>
@@ -53257,7 +53594,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="L3" s="6">
         <v>0</v>
@@ -53286,7 +53623,7 @@
     </row>
     <row r="4" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="6">
         <v>0</v>
@@ -53314,7 +53651,7 @@
         <v>0</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L4" s="6">
         <v>0</v>
@@ -53343,7 +53680,7 @@
     </row>
     <row r="5" x14ac:dyDescent="0.25">
       <c r="A5" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6">
         <v>0</v>
@@ -53371,7 +53708,7 @@
         <v>0</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L5" s="6">
         <v>0</v>
@@ -53401,7 +53738,7 @@
     </row>
     <row r="6" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" s="6">
         <v>0</v>
@@ -53429,7 +53766,7 @@
         <v>0</v>
       </c>
       <c r="K6" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="L6" s="6">
         <v>0</v>
@@ -53459,7 +53796,7 @@
     </row>
     <row r="7" x14ac:dyDescent="0.25">
       <c r="A7" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B7" s="6">
         <v>0</v>
@@ -53487,7 +53824,7 @@
         <v>0</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L7" s="6">
         <v>0</v>
@@ -53517,7 +53854,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" s="6">
         <v>0</v>
@@ -53545,7 +53882,7 @@
         <v>1.25</v>
       </c>
       <c r="K8" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="L8" s="6">
         <v>0</v>
@@ -53575,7 +53912,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.25">
       <c r="A9" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" s="6">
         <v>0</v>
@@ -53602,7 +53939,7 @@
         <v>0</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L9" s="6">
         <v>0</v>
@@ -53642,4 +53979,543 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EDF21F6-D3AE-4C9E-811B-40C24B426898}">
+  <dimension ref="A1:S9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="H1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="30" t="s">
+        <v>91</v>
+      </c>
+      <c r="L1" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q1" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="S1" s="31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" x14ac:dyDescent="0.25">
+      <c r="A2" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="4">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8">
+        <f>L_plus</f>
+        <v>3.4999999999999998E-7</v>
+      </c>
+      <c r="E2" s="8">
+        <f>L_plus*O</f>
+        <v>9.7922999999999994E-6</v>
+      </c>
+      <c r="F2" s="8">
+        <f>L_plus*O^2</f>
+        <v>2.7396896940000003E-4</v>
+      </c>
+      <c r="G2" s="8">
+        <f>L_plus*O^3</f>
+        <v>7.6651038258732001E-3</v>
+      </c>
+      <c r="H2" s="8">
+        <f>L_plus*O^4</f>
+        <v>0.2144542748402804</v>
+      </c>
+      <c r="I2" s="8">
+        <f>L_plus*O^5</f>
+        <v>6.0000017014813656</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="6">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <v>0</v>
+      </c>
+      <c r="O2" s="6">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>0</v>
+      </c>
+      <c r="D3" s="40" cm="1">
+        <f t="array" ref="D3">k_unprime_basal</f>
+        <v>0.1</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="4">
+        <v>0</v>
+      </c>
+      <c r="N3" s="41">
+        <f>-1*k_on_7</f>
+        <v>0</v>
+      </c>
+      <c r="O3" s="6">
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="6">
+        <v>0</v>
+      </c>
+      <c r="R3" s="6">
+        <v>0</v>
+      </c>
+      <c r="S3" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="34" cm="1">
+        <f t="array" ref="C4">k_prime_basal</f>
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="D4" s="32">
+        <v>0</v>
+      </c>
+      <c r="E4" s="33">
+        <f>k_off_1</f>
+        <v>4</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
+        <v>0</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>94</v>
+      </c>
+      <c r="L4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="35">
+        <f>k_on_3</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="25">
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+      <c r="R4" s="6">
+        <v>0</v>
+      </c>
+      <c r="S4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="12">
+        <f>2*b_1*k_off_1</f>
+        <v>4</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
+      </c>
+      <c r="K5" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="L5" s="6">
+        <v>0</v>
+      </c>
+      <c r="M5" s="6">
+        <v>0</v>
+      </c>
+      <c r="N5" s="13">
+        <f>5*k_on_1</f>
+        <v>700000</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="25">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+      <c r="R5" s="6">
+        <v>0</v>
+      </c>
+      <c r="S5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" x14ac:dyDescent="0.25">
+      <c r="A6" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
+        <v>0</v>
+      </c>
+      <c r="E6" s="25">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="12">
+        <f>3*b_1^2*k_off_1</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="31" t="s">
+        <v>96</v>
+      </c>
+      <c r="L6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <v>0</v>
+      </c>
+      <c r="O6" s="13">
+        <f>4*k_on_1</f>
+        <v>560000</v>
+      </c>
+      <c r="P6" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="25">
+        <v>0</v>
+      </c>
+      <c r="R6" s="6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" x14ac:dyDescent="0.25">
+      <c r="A7" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0</v>
+      </c>
+      <c r="F7" s="25">
+        <v>0</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12">
+        <f>4*b_1^3*k_off_1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="L7" s="6">
+        <v>0</v>
+      </c>
+      <c r="M7" s="6">
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6">
+        <v>0</v>
+      </c>
+      <c r="P7" s="13">
+        <f>3*k_on_1</f>
+        <v>420000</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="R7" s="25">
+        <v>0</v>
+      </c>
+      <c r="S7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="6">
+        <v>0</v>
+      </c>
+      <c r="D8" s="6">
+        <v>0</v>
+      </c>
+      <c r="E8" s="6">
+        <v>0</v>
+      </c>
+      <c r="F8" s="6">
+        <v>0</v>
+      </c>
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <f>5*b_1^4*k_off_1</f>
+        <v>1.25</v>
+      </c>
+      <c r="K8" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L8" s="6">
+        <v>0</v>
+      </c>
+      <c r="M8" s="6">
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <v>0</v>
+      </c>
+      <c r="O8" s="6">
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="13">
+        <f>2*k_on_1</f>
+        <v>280000</v>
+      </c>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+      <c r="S8" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" x14ac:dyDescent="0.25">
+      <c r="A9" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6">
+        <v>0</v>
+      </c>
+      <c r="E9" s="6">
+        <v>0</v>
+      </c>
+      <c r="F9" s="6">
+        <v>0</v>
+      </c>
+      <c r="G9" s="6">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>0</v>
+      </c>
+      <c r="I9" s="4">
+        <v>0</v>
+      </c>
+      <c r="K9" s="31" t="s">
+        <v>99</v>
+      </c>
+      <c r="L9" s="6">
+        <v>0</v>
+      </c>
+      <c r="M9" s="6">
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <v>0</v>
+      </c>
+      <c r="O9" s="6">
+        <v>0</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="6">
+        <v>0</v>
+      </c>
+      <c r="R9" s="13">
+        <f>k_on_1</f>
+        <v>140000</v>
+      </c>
+      <c r="S9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>